<commit_message>
update taskslist and meeting minutes
</commit_message>
<xml_diff>
--- a/TaskLists/EMGP Automated Car.xlsx
+++ b/TaskLists/EMGP Automated Car.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Project tasks" sheetId="1" r:id="Rbd1549720d4a4a16"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Project tasks" sheetId="1" r:id="Rce5e85acb8ff4280"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -201,7 +201,7 @@
         <x:v>% complete</x:v>
       </x:c>
       <x:c s="3">
-        <x:v>0.82</x:v>
+        <x:v>0.78</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
@@ -209,7 +209,7 @@
         <x:v>Exported on</x:v>
       </x:c>
       <x:c s="5" t="n">
-        <x:v>44658.06227875</x:v>
+        <x:v>44661.1153900463</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
@@ -603,7 +603,7 @@
         <x:v>Bucket 1</x:v>
       </x:c>
       <x:c s="1" t="str">
-        <x:v/>
+        <x:v>11 - coding, 19 - coding, 27 - coding, 35 - coding, 43 - coding</x:v>
       </x:c>
       <x:c s="1" t="str">
         <x:v/>
@@ -889,7 +889,7 @@
         <x:v>44656.4444444444</x:v>
       </x:c>
       <x:c s="1" t="str">
-        <x:v>10 - assignment of ports</x:v>
+        <x:v>10 - assignment of ports, 6 - GitHub set up</x:v>
       </x:c>
       <x:c s="3">
         <x:v>1</x:v>
@@ -1361,7 +1361,7 @@
         <x:v>44655.4444444444</x:v>
       </x:c>
       <x:c s="1" t="str">
-        <x:v>18 - assignment of ports</x:v>
+        <x:v>18 - assignment of ports, 6 - GitHub set up</x:v>
       </x:c>
       <x:c s="3">
         <x:v>1</x:v>
@@ -1833,7 +1833,7 @@
         <x:v>44655.6111111111</x:v>
       </x:c>
       <x:c s="1" t="str">
-        <x:v>26 - assignment of ports</x:v>
+        <x:v>26 - assignment of ports, 6 - GitHub set up</x:v>
       </x:c>
       <x:c s="3">
         <x:v>1</x:v>
@@ -2305,7 +2305,7 @@
         <x:v>44655.4027777778</x:v>
       </x:c>
       <x:c s="1" t="str">
-        <x:v>34 - assignment of ports</x:v>
+        <x:v>34 - assignment of ports, 6 - GitHub set up</x:v>
       </x:c>
       <x:c s="3">
         <x:v>1</x:v>
@@ -2777,6 +2777,124 @@
         <x:v>44655.4027777778</x:v>
       </x:c>
       <x:c s="1" t="str">
+        <x:v>42 - assignment of ports, 6 - GitHub set up</x:v>
+      </x:c>
+      <x:c s="3">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Bucket 1</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>44 - unit testing</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>4 hours</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>4 hours</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>0 hours</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>No</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="53">
+      <x:c s="1" t="n">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>11.5</x:v>
+      </x:c>
+      <x:c s="11" t="str">
+        <x:v>unit testing</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Lily Zhang</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>4 hours</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44655.4027777778</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44655.5694444444</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>43 - coding</x:v>
+      </x:c>
+      <x:c s="3">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Bucket 1</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>48 - Integration of all the interfaces, 46 - code review</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>4 hours</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>4 hours</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>0 hours</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>No</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="54">
+      <x:c s="1" t="n">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>11.6</x:v>
+      </x:c>
+      <x:c s="11" t="str">
+        <x:v>hardware team review</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>4 hours</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44652.5694444444</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44655.4027777778</x:v>
+      </x:c>
+      <x:c s="1" t="str">
         <x:v>42 - assignment of ports</x:v>
       </x:c>
       <x:c s="3">
@@ -2786,13 +2904,131 @@
         <x:v>Bucket 1</x:v>
       </x:c>
       <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>No</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="55">
+      <x:c s="1" t="n">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>11.7</x:v>
+      </x:c>
+      <x:c s="11" t="str">
+        <x:v>code review</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>4 hours</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44655.5694444444</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44656.4027777778</x:v>
+      </x:c>
+      <x:c s="1" t="str">
         <x:v>44 - unit testing</x:v>
       </x:c>
-      <x:c s="1" t="str">
-        <x:v>4 hours</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>4 hours</x:v>
+      <x:c s="3">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Bucket 1</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>No</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="56">
+      <x:c s="1" t="n">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Integration of all components</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Cher Khor</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>2 hours</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44655.4444444444</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44655.5277777778</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>34 - assignment of ports, 26 - assignment of ports, 42 - assignment of ports, 18 - assignment of ports, 10 - assignment of ports</x:v>
+      </x:c>
+      <x:c s="3">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Bucket 1</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>2 hours</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>2 hours</x:v>
       </x:c>
       <x:c s="1" t="str">
         <x:v>0 hours</x:v>
@@ -2813,45 +3049,45 @@
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="53">
-      <x:c s="1" t="n">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>11.5</x:v>
-      </x:c>
-      <x:c s="11" t="str">
-        <x:v>unit testing</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>Lily Zhang</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>4 hours</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44655.4027777778</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44655.5694444444</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>43 - coding</x:v>
-      </x:c>
-      <x:c s="3">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>Bucket 1</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>48 - Integration of all the interfaces, 46 - code review</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>4 hours</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>4 hours</x:v>
+    <x:row r="57">
+      <x:c s="1" t="n">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Integration of all the interfaces</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Thomas Le</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>8 hours</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44657.4444444444</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44658.4444444444</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>44 - unit testing, 36 - unit testing, 28 - unit testing, 20 - unit testing, 12 - unit testing</x:v>
+      </x:c>
+      <x:c s="3">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Bucket 1</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>49 - Car Mount</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>8 hours</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>8 hours</x:v>
       </x:c>
       <x:c s="1" t="str">
         <x:v>0 hours</x:v>
@@ -2872,242 +3108,6 @@
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="54">
-      <x:c s="1" t="n">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>11.6</x:v>
-      </x:c>
-      <x:c s="11" t="str">
-        <x:v>hardware team review</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>4 hours</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44652.5694444444</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44655.4027777778</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>42 - assignment of ports</x:v>
-      </x:c>
-      <x:c s="3">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>Bucket 1</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>No</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="55">
-      <x:c s="1" t="n">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>11.7</x:v>
-      </x:c>
-      <x:c s="11" t="str">
-        <x:v>code review</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>4 hours</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44655.5694444444</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44656.4027777778</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>44 - unit testing</x:v>
-      </x:c>
-      <x:c s="3">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>Bucket 1</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>No</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="56">
-      <x:c s="1" t="n">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>Integration of all components</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>Cher Khor</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>2 hours</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44655.4444444444</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44655.5277777778</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>34 - assignment of ports, 26 - assignment of ports, 42 - assignment of ports, 18 - assignment of ports, 10 - assignment of ports</x:v>
-      </x:c>
-      <x:c s="3">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>Bucket 1</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>2 hours</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>0 hours</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>2 hours</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>No</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="57">
-      <x:c s="1" t="n">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>Integration of all the interfaces</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>Thomas Le</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>8 hours</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44657.4444444444</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44658.4444444444</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>44 - unit testing, 36 - unit testing, 28 - unit testing, 20 - unit testing, 12 - unit testing</x:v>
-      </x:c>
-      <x:c s="3">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>Bucket 1</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>8 hours</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>0 hours</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>8 hours</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>No</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-    </x:row>
     <x:row r="58">
       <x:c s="1" t="n">
         <x:v>49</x:v>
@@ -3131,7 +3131,66 @@
         <x:v>44649.7083333333</x:v>
       </x:c>
       <x:c s="1" t="str">
-        <x:v/>
+        <x:v>48 - Integration of all the interfaces</x:v>
+      </x:c>
+      <x:c s="3">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Bucket 1</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>50 - Report + log book</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>No</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="59">
+      <x:c s="1" t="n">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Report + log book</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>5 days</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44650.375</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44656.7083333333</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>49 - Car Mount</x:v>
       </x:c>
       <x:c s="3">
         <x:v>0</x:v>

</xml_diff>

<commit_message>
update minute and task list
</commit_message>
<xml_diff>
--- a/TaskLists/EMGP Automated Car.xlsx
+++ b/TaskLists/EMGP Automated Car.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Project tasks" sheetId="1" r:id="Rce5e85acb8ff4280"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Project tasks" sheetId="1" r:id="Radc865ebf8ac47cf"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -185,7 +185,7 @@
         <x:v>Project finish date</x:v>
       </x:c>
       <x:c s="5" t="n">
-        <x:v>44658.4444444444</x:v>
+        <x:v>44672.7083333333</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -193,7 +193,7 @@
         <x:v>Duration</x:v>
       </x:c>
       <x:c s="1" t="str">
-        <x:v>8.21 days</x:v>
+        <x:v>19 days</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
@@ -201,7 +201,7 @@
         <x:v>% complete</x:v>
       </x:c>
       <x:c s="3">
-        <x:v>0.78</x:v>
+        <x:v>0.67</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
@@ -209,7 +209,7 @@
         <x:v>Exported on</x:v>
       </x:c>
       <x:c s="5" t="n">
-        <x:v>44661.1153900463</x:v>
+        <x:v>44670.4002092593</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
@@ -898,7 +898,7 @@
         <x:v>Bucket 1</x:v>
       </x:c>
       <x:c s="1" t="str">
-        <x:v>12 - unit testing</x:v>
+        <x:v>12 - unit testing, 13 - hardware team review</x:v>
       </x:c>
       <x:c s="1" t="str">
         <x:v>8 hours</x:v>
@@ -1007,7 +1007,7 @@
         <x:v>44655.6111111111</x:v>
       </x:c>
       <x:c s="1" t="str">
-        <x:v>10 - assignment of ports</x:v>
+        <x:v>10 - assignment of ports, 11 - coding</x:v>
       </x:c>
       <x:c s="3">
         <x:v>1</x:v>
@@ -1470,10 +1470,10 @@
         <x:v/>
       </x:c>
       <x:c s="1" t="str">
-        <x:v>4 hours</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44652.6111111111</x:v>
+        <x:v>1.67 hours</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44655.375</x:v>
       </x:c>
       <x:c s="5" t="n">
         <x:v>44655.4444444444</x:v>
@@ -1588,13 +1588,13 @@
         <x:v/>
       </x:c>
       <x:c s="2" t="str">
-        <x:v>2.94 days</x:v>
+        <x:v>3.94 days</x:v>
       </x:c>
       <x:c s="6" t="n">
         <x:v>44652.4652777778</x:v>
       </x:c>
       <x:c s="6" t="n">
-        <x:v>44657.4444444444</x:v>
+        <x:v>44658.4444444444</x:v>
       </x:c>
       <x:c s="2" t="str">
         <x:v>4 - Inventory</x:v>
@@ -2004,10 +2004,10 @@
         <x:v>4 hours</x:v>
       </x:c>
       <x:c s="5" t="n">
-        <x:v>44656.6111111111</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44657.4444444444</x:v>
+        <x:v>44657.6111111111</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44658.4444444444</x:v>
       </x:c>
       <x:c s="1" t="str">
         <x:v>28 - unit testing</x:v>
@@ -3022,7 +3022,7 @@
         <x:v>Bucket 1</x:v>
       </x:c>
       <x:c s="1" t="str">
-        <x:v/>
+        <x:v>49 - Car Mount</x:v>
       </x:c>
       <x:c s="1" t="str">
         <x:v>2 hours</x:v>
@@ -3125,13 +3125,13 @@
         <x:v>16 hours</x:v>
       </x:c>
       <x:c s="5" t="n">
-        <x:v>44648.375</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44649.7083333333</x:v>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v>48 - Integration of all the interfaces</x:v>
+        <x:v>44658.375</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44659.7083333333</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>48 - Integration of all the interfaces, 47 - Integration of all components</x:v>
       </x:c>
       <x:c s="3">
         <x:v>1</x:v>
@@ -3181,13 +3181,13 @@
         <x:v/>
       </x:c>
       <x:c s="1" t="str">
-        <x:v>5 days</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44650.375</x:v>
-      </x:c>
-      <x:c s="5" t="n">
-        <x:v>44656.7083333333</x:v>
+        <x:v>6 days</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44662.375</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44669.7083333333</x:v>
       </x:c>
       <x:c s="1" t="str">
         <x:v>49 - Car Mount</x:v>
@@ -3199,16 +3199,75 @@
         <x:v>Bucket 1</x:v>
       </x:c>
       <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
-      </x:c>
-      <x:c s="1" t="str">
-        <x:v/>
+        <x:v>51 - Poster</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>No</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="60">
+      <x:c s="1" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Poster</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Cher Khor</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>3 days</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44670.375</x:v>
+      </x:c>
+      <x:c s="5" t="n">
+        <x:v>44672.7083333333</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>50 - Report + log book</x:v>
+      </x:c>
+      <x:c s="3">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Bucket 1</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>24 hours</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>0 hours</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>24 hours</x:v>
       </x:c>
       <x:c s="1" t="str">
         <x:v>No</x:v>

</xml_diff>